<commit_message>
HWs and Class Work
</commit_message>
<xml_diff>
--- a/HW3/dotProd_Data_Analysis.xlsx
+++ b/HW3/dotProd_Data_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasongraalum/PSU/CS531_Winter_2019/HW3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27161A77-763F-5640-864F-C2395A12BF9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96B763-A972-F941-814F-F665A2E9A86D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="35500" windowHeight="17040" xr2:uid="{D9AF792A-9D93-FC43-B460-65539082BC33}"/>
+    <workbookView xWindow="2520" yWindow="1560" windowWidth="35500" windowHeight="17040" xr2:uid="{D9AF792A-9D93-FC43-B460-65539082BC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,9 @@
     <sheet name="Run 3 " sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Run 1'!$B$1:$B$30</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Run 2'!$B$1:$B$30</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Run 2'!$B$1:$B$30</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Run 3 '!$B$3:$B$302</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Run 3 '!$B$3:$B$32</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Run 3 '!$B$3:$B$302</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Run 3 '!$H$3:$H$302</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Run 3 '!$B$3:$B$302</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Run 3 '!$B$3:$B$302</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Run 3 '!$H$3:$H$302</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -170,7 +166,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -186,10 +182,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
+            <a:defRPr sz="2400"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -234,7 +230,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -250,10 +246,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
+            <a:defRPr sz="2400"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -1471,15 +1467,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>393700</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1515,8 +1511,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8394700" y="9931400"/>
-              <a:ext cx="9918700" cy="5518150"/>
+              <a:off x="8255000" y="9944100"/>
+              <a:ext cx="10299700" cy="5518150"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1544,6 +1540,266 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A37287C-BCB5-AC4C-A64E-DCF718CC7EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18199100" y="15062200"/>
+          <a:ext cx="342900" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C07AADAB-BE7E-4844-A909-F36A6D71020B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17411700" y="14668500"/>
+          <a:ext cx="1168400" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Outlier</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048256E8-C850-C34E-BA47-D1C8B2C5CD09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17475200" y="8851900"/>
+          <a:ext cx="1168400" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Outlier</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Oval 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C92A0EDB-F7C8-8C4D-BDFE-56E50A8B5C97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18478500" y="9105900"/>
+          <a:ext cx="342900" cy="673100"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1846,10 +2102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241EF1E1-56E0-244D-B559-5B4CCA697AF0}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2474,7 +2730,7 @@
         <v>254.33007786289679</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2482,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1.96</v>
       </c>
@@ -2506,7 +2762,7 @@
         <v>91.010849522401855</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>SQRT(30)</f>
         <v>5.4772255750516612</v>
@@ -2516,7 +2772,7 @@
         <v>5.4772255750516612</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B39">
         <f>B31</f>
         <v>1130.7</v>
@@ -2540,12 +2796,12 @@
         <v>91.010849522401855</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2574,7 +2830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -2609,7 +2865,7 @@
         <v>41.126936138331985</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2643,8 +2899,12 @@
         <f>H47-G47</f>
         <v>152.76821169831737</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <f>POWER(1.96*F47/(0.05*E47),2)</f>
+        <v>49.289012347453159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -3774,8 +4034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06C942D-F6AB-8247-8EEB-6FF0A0A6A1BA}">
   <dimension ref="A1:U302"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>